<commit_message>
Updated the excel time binning file and explained how I binned the data.
</commit_message>
<xml_diff>
--- a/Sensor and Component Tests/Sound Sensor Tests /Sound sensor test 03192025 /Data analysis 05172025/Binning test.xlsx
+++ b/Sensor and Component Tests/Sound Sensor Tests /Sound sensor test 03192025 /Data analysis 05172025/Binning test.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10511"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kriishhate/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kriishhate/GitHub/CommonSENSES/Sensor and Component Tests/Sound Sensor Tests /Sound sensor test 03192025 /Data analysis 05172025/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E45AE4C-FA7D-4B4B-8B8E-759217120983}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6FF019D-A6AD-B445-83AF-13EEAA427FBB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3040" yWindow="1220" windowWidth="28040" windowHeight="17440" activeTab="1" xr2:uid="{0E5BB330-E587-0947-824C-79325281CD17}"/>
   </bookViews>
@@ -17,9 +17,9 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="7" r:id="rId4"/>
+    <pivotCache cacheId="0" r:id="rId4"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="16">
   <si>
     <t>Timestamp</t>
   </si>
@@ -72,12 +72,50 @@
   <si>
     <t>Average of Sensor3_ADC</t>
   </si>
+  <si>
+    <t xml:space="preserve">FLOOR(30317, 10) → </t>
+  </si>
+  <si>
+    <t xml:space="preserve">→ 30317 ÷ 10 = 3031.7  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">→ cut off the decimal → 3031  </t>
+  </si>
+  <si>
+    <t>→ 3031 × 10 = 30310</t>
+  </si>
+  <si>
+    <t>To figure that out, we look for the largest number that is a multiple of 10 and still smaller than or equal to 30317.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">The formula </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>FLOOR(Timestamp, 100)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> takes each timestamp and rounds it down to the nearest multiple of 10.</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -99,6 +137,18 @@
       <color theme="1"/>
       <name val="Aptos Narrow"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -127,11 +177,11 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3267,7 +3317,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{35C9B63F-C37A-0446-9ACE-27F735E40A09}" name="PivotTable2" cacheId="7" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{35C9B63F-C37A-0446-9ACE-27F735E40A09}" name="PivotTable2" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
   <location ref="A1:D46" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="5">
     <pivotField showAll="0"/>
@@ -3854,7 +3904,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="3" t="s">
         <v>5</v>
       </c>
       <c r="B1" t="s">
@@ -3868,632 +3918,632 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="5">
+      <c r="A2" s="4">
         <v>30000</v>
       </c>
-      <c r="B2" s="3">
+      <c r="B2">
         <v>8630.75</v>
       </c>
-      <c r="C2" s="3">
+      <c r="C2">
         <v>8863.25</v>
       </c>
-      <c r="D2" s="3">
+      <c r="D2">
         <v>8779.25</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="5">
+      <c r="A3" s="4">
         <v>30100</v>
       </c>
-      <c r="B3" s="3">
+      <c r="B3">
         <v>8758</v>
       </c>
-      <c r="C3" s="3">
+      <c r="C3">
         <v>8969.3333333333339</v>
       </c>
-      <c r="D3" s="3">
+      <c r="D3">
         <v>8978</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" s="5">
+      <c r="A4" s="4">
         <v>30200</v>
       </c>
-      <c r="B4" s="3">
+      <c r="B4">
         <v>8795.5</v>
       </c>
-      <c r="C4" s="3">
+      <c r="C4">
         <v>8992.5</v>
       </c>
-      <c r="D4" s="3">
+      <c r="D4">
         <v>9018</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" s="5">
+      <c r="A5" s="4">
         <v>30300</v>
       </c>
-      <c r="B5" s="3">
+      <c r="B5">
         <v>8689</v>
       </c>
-      <c r="C5" s="3">
+      <c r="C5">
         <v>8955.75</v>
       </c>
-      <c r="D5" s="3">
+      <c r="D5">
         <v>8904.75</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" s="5">
+      <c r="A6" s="4">
         <v>30400</v>
       </c>
-      <c r="B6" s="3">
+      <c r="B6">
         <v>8566.5</v>
       </c>
-      <c r="C6" s="3">
+      <c r="C6">
         <v>8859</v>
       </c>
-      <c r="D6" s="3">
+      <c r="D6">
         <v>8892</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" s="5">
+      <c r="A7" s="4">
         <v>30500</v>
       </c>
-      <c r="B7" s="3">
+      <c r="B7">
         <v>8751</v>
       </c>
-      <c r="C7" s="3">
+      <c r="C7">
         <v>8977.75</v>
       </c>
-      <c r="D7" s="3">
+      <c r="D7">
         <v>8970.75</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" s="5">
+      <c r="A8" s="4">
         <v>30600</v>
       </c>
-      <c r="B8" s="3">
+      <c r="B8">
         <v>8601.75</v>
       </c>
-      <c r="C8" s="3">
+      <c r="C8">
         <v>8804.75</v>
       </c>
-      <c r="D8" s="3">
+      <c r="D8">
         <v>8919</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" s="5">
+      <c r="A9" s="4">
         <v>30700</v>
       </c>
-      <c r="B9" s="3">
+      <c r="B9">
         <v>8746.3333333333339</v>
       </c>
-      <c r="C9" s="3">
+      <c r="C9">
         <v>8989.3333333333339</v>
       </c>
-      <c r="D9" s="3">
+      <c r="D9">
         <v>9005.6666666666661</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" s="5">
+      <c r="A10" s="4">
         <v>30800</v>
       </c>
-      <c r="B10" s="3">
+      <c r="B10">
         <v>8842.25</v>
       </c>
-      <c r="C10" s="3">
+      <c r="C10">
         <v>9078</v>
       </c>
-      <c r="D10" s="3">
+      <c r="D10">
         <v>9038.75</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11" s="5">
+      <c r="A11" s="4">
         <v>30900</v>
       </c>
-      <c r="B11" s="3">
+      <c r="B11">
         <v>8907</v>
       </c>
-      <c r="C11" s="3">
+      <c r="C11">
         <v>9152</v>
       </c>
-      <c r="D11" s="3">
+      <c r="D11">
         <v>9085.6666666666661</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A12" s="5">
+      <c r="A12" s="4">
         <v>31000</v>
       </c>
-      <c r="B12" s="3">
+      <c r="B12">
         <v>8917</v>
       </c>
-      <c r="C12" s="3">
+      <c r="C12">
         <v>9150.6666666666661</v>
       </c>
-      <c r="D12" s="3">
+      <c r="D12">
         <v>9191.3333333333339</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A13" s="5">
+      <c r="A13" s="4">
         <v>31100</v>
       </c>
-      <c r="B13" s="3">
+      <c r="B13">
         <v>8641.75</v>
       </c>
-      <c r="C13" s="3">
+      <c r="C13">
         <v>8939</v>
       </c>
-      <c r="D13" s="3">
+      <c r="D13">
         <v>9013.75</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A14" s="5">
+      <c r="A14" s="4">
         <v>31200</v>
       </c>
-      <c r="B14" s="3">
+      <c r="B14">
         <v>8493.5</v>
       </c>
-      <c r="C14" s="3">
+      <c r="C14">
         <v>8765</v>
       </c>
-      <c r="D14" s="3">
+      <c r="D14">
         <v>8807</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A15" s="5">
+      <c r="A15" s="4">
         <v>31300</v>
       </c>
-      <c r="B15" s="3">
+      <c r="B15">
         <v>8480.6666666666661</v>
       </c>
-      <c r="C15" s="3">
+      <c r="C15">
         <v>8785</v>
       </c>
-      <c r="D15" s="3">
+      <c r="D15">
         <v>8752</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A16" s="5">
+      <c r="A16" s="4">
         <v>31400</v>
       </c>
-      <c r="B16" s="3">
+      <c r="B16">
         <v>8518.6666666666661</v>
       </c>
-      <c r="C16" s="3">
+      <c r="C16">
         <v>8808.3333333333339</v>
       </c>
-      <c r="D16" s="3">
+      <c r="D16">
         <v>8748</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A17" s="5">
+      <c r="A17" s="4">
         <v>31500</v>
       </c>
-      <c r="B17" s="3">
+      <c r="B17">
         <v>8485.75</v>
       </c>
-      <c r="C17" s="3">
+      <c r="C17">
         <v>8752.75</v>
       </c>
-      <c r="D17" s="3">
+      <c r="D17">
         <v>8808.25</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A18" s="5">
+      <c r="A18" s="4">
         <v>31600</v>
       </c>
-      <c r="B18" s="3">
+      <c r="B18">
         <v>8537</v>
       </c>
-      <c r="C18" s="3">
+      <c r="C18">
         <v>8791.3333333333339</v>
       </c>
-      <c r="D18" s="3">
+      <c r="D18">
         <v>8779.6666666666661</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A19" s="5">
+      <c r="A19" s="4">
         <v>31700</v>
       </c>
-      <c r="B19" s="3">
+      <c r="B19">
         <v>8523.25</v>
       </c>
-      <c r="C19" s="3">
+      <c r="C19">
         <v>8761.25</v>
       </c>
-      <c r="D19" s="3">
+      <c r="D19">
         <v>8749</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A20" s="5">
+      <c r="A20" s="4">
         <v>31800</v>
       </c>
-      <c r="B20" s="3">
+      <c r="B20">
         <v>8491.25</v>
       </c>
-      <c r="C20" s="3">
+      <c r="C20">
         <v>8700.5</v>
       </c>
-      <c r="D20" s="3">
+      <c r="D20">
         <v>8668.5</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A21" s="5">
+      <c r="A21" s="4">
         <v>31900</v>
       </c>
-      <c r="B21" s="3">
+      <c r="B21">
         <v>8478.3333333333339</v>
       </c>
-      <c r="C21" s="3">
+      <c r="C21">
         <v>8714</v>
       </c>
-      <c r="D21" s="3">
+      <c r="D21">
         <v>8769</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A22" s="5">
+      <c r="A22" s="4">
         <v>32000</v>
       </c>
-      <c r="B22" s="3">
+      <c r="B22">
         <v>8411.3333333333339</v>
       </c>
-      <c r="C22" s="3">
+      <c r="C22">
         <v>8671</v>
       </c>
-      <c r="D22" s="3">
+      <c r="D22">
         <v>8748.3333333333339</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A23" s="5">
+      <c r="A23" s="4">
         <v>32100</v>
       </c>
-      <c r="B23" s="3">
+      <c r="B23">
         <v>8581.75</v>
       </c>
-      <c r="C23" s="3">
+      <c r="C23">
         <v>8820</v>
       </c>
-      <c r="D23" s="3">
+      <c r="D23">
         <v>8768.5</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A24" s="5">
+      <c r="A24" s="4">
         <v>32200</v>
       </c>
-      <c r="B24" s="3">
+      <c r="B24">
         <v>8676</v>
       </c>
-      <c r="C24" s="3">
+      <c r="C24">
         <v>8906.3333333333339</v>
       </c>
-      <c r="D24" s="3">
+      <c r="D24">
         <v>8866.6666666666661</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A25" s="5">
+      <c r="A25" s="4">
         <v>32300</v>
       </c>
-      <c r="B25" s="3">
+      <c r="B25">
         <v>8483.75</v>
       </c>
-      <c r="C25" s="3">
+      <c r="C25">
         <v>8872.25</v>
       </c>
-      <c r="D25" s="3">
+      <c r="D25">
         <v>8850.25</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A26" s="5">
+      <c r="A26" s="4">
         <v>32400</v>
       </c>
-      <c r="B26" s="3">
+      <c r="B26">
         <v>8741.3333333333339</v>
       </c>
-      <c r="C26" s="3">
+      <c r="C26">
         <v>8943</v>
       </c>
-      <c r="D26" s="3">
+      <c r="D26">
         <v>8974.6666666666661</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A27" s="5">
+      <c r="A27" s="4">
         <v>32500</v>
       </c>
-      <c r="B27" s="3">
+      <c r="B27">
         <v>8633.3333333333339</v>
       </c>
-      <c r="C27" s="3">
+      <c r="C27">
         <v>8918</v>
       </c>
-      <c r="D27" s="3">
+      <c r="D27">
         <v>8887.3333333333339</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A28" s="5">
+      <c r="A28" s="4">
         <v>32600</v>
       </c>
-      <c r="B28" s="3">
+      <c r="B28">
         <v>8523.25</v>
       </c>
-      <c r="C28" s="3">
+      <c r="C28">
         <v>8777</v>
       </c>
-      <c r="D28" s="3">
+      <c r="D28">
         <v>8760.25</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A29" s="5">
+      <c r="A29" s="4">
         <v>32700</v>
       </c>
-      <c r="B29" s="3">
+      <c r="B29">
         <v>8660</v>
       </c>
-      <c r="C29" s="3">
+      <c r="C29">
         <v>8835.3333333333339</v>
       </c>
-      <c r="D29" s="3">
+      <c r="D29">
         <v>8877.6666666666661</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A30" s="5">
+      <c r="A30" s="4">
         <v>32800</v>
       </c>
-      <c r="B30" s="3">
+      <c r="B30">
         <v>8746.75</v>
       </c>
-      <c r="C30" s="3">
+      <c r="C30">
         <v>8936</v>
       </c>
-      <c r="D30" s="3">
+      <c r="D30">
         <v>8975.5</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A31" s="5">
+      <c r="A31" s="4">
         <v>32900</v>
       </c>
-      <c r="B31" s="3">
+      <c r="B31">
         <v>8564.6666666666661</v>
       </c>
-      <c r="C31" s="3">
+      <c r="C31">
         <v>8817.6666666666661</v>
       </c>
-      <c r="D31" s="3">
+      <c r="D31">
         <v>8870.3333333333339</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A32" s="5">
+      <c r="A32" s="4">
         <v>33000</v>
       </c>
-      <c r="B32" s="3">
+      <c r="B32">
         <v>8611.6666666666661</v>
       </c>
-      <c r="C32" s="3">
+      <c r="C32">
         <v>8792.6666666666661</v>
       </c>
-      <c r="D32" s="3">
+      <c r="D32">
         <v>8915</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A33" s="5">
+      <c r="A33" s="4">
         <v>33100</v>
       </c>
-      <c r="B33" s="3">
+      <c r="B33">
         <v>8637.25</v>
       </c>
-      <c r="C33" s="3">
+      <c r="C33">
         <v>8894.25</v>
       </c>
-      <c r="D33" s="3">
+      <c r="D33">
         <v>8889.5</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A34" s="5">
+      <c r="A34" s="4">
         <v>33200</v>
       </c>
-      <c r="B34" s="3">
+      <c r="B34">
         <v>8538</v>
       </c>
-      <c r="C34" s="3">
+      <c r="C34">
         <v>8781</v>
       </c>
-      <c r="D34" s="3">
+      <c r="D34">
         <v>8773</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A35" s="5">
+      <c r="A35" s="4">
         <v>33300</v>
       </c>
-      <c r="B35" s="3">
+      <c r="B35">
         <v>8557</v>
       </c>
-      <c r="C35" s="3">
+      <c r="C35">
         <v>8773</v>
       </c>
-      <c r="D35" s="3">
+      <c r="D35">
         <v>8778.6666666666661</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A36" s="5">
+      <c r="A36" s="4">
         <v>33400</v>
       </c>
-      <c r="B36" s="3">
+      <c r="B36">
         <v>8594.3333333333339</v>
       </c>
-      <c r="C36" s="3">
+      <c r="C36">
         <v>8862.6666666666661</v>
       </c>
-      <c r="D36" s="3">
+      <c r="D36">
         <v>8856.6666666666661</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A37" s="5">
+      <c r="A37" s="4">
         <v>33500</v>
       </c>
-      <c r="B37" s="3">
+      <c r="B37">
         <v>8548.25</v>
       </c>
-      <c r="C37" s="3">
+      <c r="C37">
         <v>8858.5</v>
       </c>
-      <c r="D37" s="3">
+      <c r="D37">
         <v>8879.5</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A38" s="5">
+      <c r="A38" s="4">
         <v>33600</v>
       </c>
-      <c r="B38" s="3">
+      <c r="B38">
         <v>8617</v>
       </c>
-      <c r="C38" s="3">
+      <c r="C38">
         <v>8904.3333333333339</v>
       </c>
-      <c r="D38" s="3">
+      <c r="D38">
         <v>8905.6666666666661</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A39" s="5">
+      <c r="A39" s="4">
         <v>33700</v>
       </c>
-      <c r="B39" s="3">
+      <c r="B39">
         <v>8699.25</v>
       </c>
-      <c r="C39" s="3">
+      <c r="C39">
         <v>8835.25</v>
       </c>
-      <c r="D39" s="3">
+      <c r="D39">
         <v>9580</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A40" s="5">
+      <c r="A40" s="4">
         <v>33800</v>
       </c>
-      <c r="B40" s="3">
+      <c r="B40">
         <v>12269.75</v>
       </c>
-      <c r="C40" s="3">
+      <c r="C40">
         <v>12348.5</v>
       </c>
-      <c r="D40" s="3">
+      <c r="D40">
         <v>12215</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A41" s="5">
+      <c r="A41" s="4">
         <v>33900</v>
       </c>
-      <c r="B41" s="3">
+      <c r="B41">
         <v>11024.333333333334</v>
       </c>
-      <c r="C41" s="3">
+      <c r="C41">
         <v>11244.666666666666</v>
       </c>
-      <c r="D41" s="3">
+      <c r="D41">
         <v>11199.333333333334</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A42" s="5">
+      <c r="A42" s="4">
         <v>34000</v>
       </c>
-      <c r="B42" s="3">
+      <c r="B42">
         <v>9964.6666666666661</v>
       </c>
-      <c r="C42" s="3">
+      <c r="C42">
         <v>10324.666666666666</v>
       </c>
-      <c r="D42" s="3">
+      <c r="D42">
         <v>10109.333333333334</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A43" s="5">
+      <c r="A43" s="4">
         <v>34100</v>
       </c>
-      <c r="B43" s="3">
+      <c r="B43">
         <v>8872.5</v>
       </c>
-      <c r="C43" s="3">
+      <c r="C43">
         <v>9451.75</v>
       </c>
-      <c r="D43" s="3">
+      <c r="D43">
         <v>9386.5</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A44" s="5">
+      <c r="A44" s="4">
         <v>34200</v>
       </c>
-      <c r="B44" s="3">
+      <c r="B44">
         <v>8082.666666666667</v>
       </c>
-      <c r="C44" s="3">
+      <c r="C44">
         <v>8662</v>
       </c>
-      <c r="D44" s="3">
+      <c r="D44">
         <v>8630.3333333333339</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A45" s="5">
+      <c r="A45" s="4">
         <v>34300</v>
       </c>
-      <c r="B45" s="3">
+      <c r="B45">
         <v>8244</v>
       </c>
-      <c r="C45" s="3">
+      <c r="C45">
         <v>8498</v>
       </c>
-      <c r="D45" s="3">
+      <c r="D45">
         <v>8448</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A46" s="5" t="s">
+      <c r="A46" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B46" s="3">
+      <c r="B46">
         <v>8788.0400000000009</v>
       </c>
-      <c r="C46" s="3">
+      <c r="C46">
         <v>9046.1466666666674</v>
       </c>
-      <c r="D46" s="3">
+      <c r="D46">
         <v>9060.2666666666664</v>
       </c>
     </row>
@@ -4505,15 +4555,18 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4570627F-1661-A241-AF43-CA9AE7F7284C}">
-  <dimension ref="A1:E151"/>
+  <dimension ref="A1:G151"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="7" max="7" width="89" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4530,7 +4583,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>30003</v>
       </c>
@@ -4547,8 +4600,11 @@
         <f>FLOOR(A2, 100)</f>
         <v>30000</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G2" s="5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>30029</v>
       </c>
@@ -4565,8 +4621,11 @@
         <f t="shared" ref="E3:E66" si="0">FLOOR(A3, 100)</f>
         <v>30000</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G3" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>30056</v>
       </c>
@@ -4583,8 +4642,11 @@
         <f t="shared" si="0"/>
         <v>30000</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G4" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>30083</v>
       </c>
@@ -4601,8 +4663,11 @@
         <f t="shared" si="0"/>
         <v>30000</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G5" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>30109</v>
       </c>
@@ -4619,8 +4684,11 @@
         <f t="shared" si="0"/>
         <v>30100</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G6" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>30136</v>
       </c>
@@ -4637,8 +4705,11 @@
         <f t="shared" si="0"/>
         <v>30100</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G7" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>30162</v>
       </c>
@@ -4656,7 +4727,7 @@
         <v>30100</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>30211</v>
       </c>
@@ -4674,7 +4745,7 @@
         <v>30200</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>30237</v>
       </c>
@@ -4692,7 +4763,7 @@
         <v>30200</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>30264</v>
       </c>
@@ -4710,7 +4781,7 @@
         <v>30200</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>30290</v>
       </c>
@@ -4728,7 +4799,7 @@
         <v>30200</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>30317</v>
       </c>
@@ -4746,7 +4817,7 @@
         <v>30300</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>30344</v>
       </c>
@@ -4764,7 +4835,7 @@
         <v>30300</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>30370</v>
       </c>
@@ -4782,7 +4853,7 @@
         <v>30300</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>30397</v>
       </c>
@@ -7257,362 +7328,362 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" s="3">
+      <c r="A2">
         <v>8630.75</v>
       </c>
-      <c r="B2" s="3">
+      <c r="B2">
         <v>8863.25</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" s="3">
+      <c r="A3">
         <v>8758</v>
       </c>
-      <c r="B3" s="3">
+      <c r="B3">
         <v>8969.3333333333339</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" s="3">
+      <c r="A4">
         <v>8795.5</v>
       </c>
-      <c r="B4" s="3">
+      <c r="B4">
         <v>8992.5</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" s="3">
+      <c r="A5">
         <v>8689</v>
       </c>
-      <c r="B5" s="3">
+      <c r="B5">
         <v>8955.75</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" s="3">
+      <c r="A6">
         <v>8566.5</v>
       </c>
-      <c r="B6" s="3">
+      <c r="B6">
         <v>8859</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" s="3">
+      <c r="A7">
         <v>8751</v>
       </c>
-      <c r="B7" s="3">
+      <c r="B7">
         <v>8977.75</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A8" s="3">
+      <c r="A8">
         <v>8601.75</v>
       </c>
-      <c r="B8" s="3">
+      <c r="B8">
         <v>8804.75</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A9" s="3">
+      <c r="A9">
         <v>8746.3333333333339</v>
       </c>
-      <c r="B9" s="3">
+      <c r="B9">
         <v>8989.3333333333339</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A10" s="3">
+      <c r="A10">
         <v>8842.25</v>
       </c>
-      <c r="B10" s="3">
+      <c r="B10">
         <v>9078</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A11" s="3">
+      <c r="A11">
         <v>8907</v>
       </c>
-      <c r="B11" s="3">
+      <c r="B11">
         <v>9152</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A12" s="3">
+      <c r="A12">
         <v>8917</v>
       </c>
-      <c r="B12" s="3">
+      <c r="B12">
         <v>9150.6666666666661</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A13" s="3">
+      <c r="A13">
         <v>8641.75</v>
       </c>
-      <c r="B13" s="3">
+      <c r="B13">
         <v>8939</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A14" s="3">
+      <c r="A14">
         <v>8493.5</v>
       </c>
-      <c r="B14" s="3">
+      <c r="B14">
         <v>8765</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A15" s="3">
+      <c r="A15">
         <v>8480.6666666666661</v>
       </c>
-      <c r="B15" s="3">
+      <c r="B15">
         <v>8785</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A16" s="3">
+      <c r="A16">
         <v>8518.6666666666661</v>
       </c>
-      <c r="B16" s="3">
+      <c r="B16">
         <v>8808.3333333333339</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A17" s="3">
+      <c r="A17">
         <v>8485.75</v>
       </c>
-      <c r="B17" s="3">
+      <c r="B17">
         <v>8752.75</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A18" s="3">
+      <c r="A18">
         <v>8537</v>
       </c>
-      <c r="B18" s="3">
+      <c r="B18">
         <v>8791.3333333333339</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A19" s="3">
+      <c r="A19">
         <v>8523.25</v>
       </c>
-      <c r="B19" s="3">
+      <c r="B19">
         <v>8761.25</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A20" s="3">
+      <c r="A20">
         <v>8491.25</v>
       </c>
-      <c r="B20" s="3">
+      <c r="B20">
         <v>8700.5</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A21" s="3">
+      <c r="A21">
         <v>8478.3333333333339</v>
       </c>
-      <c r="B21" s="3">
+      <c r="B21">
         <v>8714</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A22" s="3">
+      <c r="A22">
         <v>8411.3333333333339</v>
       </c>
-      <c r="B22" s="3">
+      <c r="B22">
         <v>8671</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A23" s="3">
+      <c r="A23">
         <v>8581.75</v>
       </c>
-      <c r="B23" s="3">
+      <c r="B23">
         <v>8820</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A24" s="3">
+      <c r="A24">
         <v>8676</v>
       </c>
-      <c r="B24" s="3">
+      <c r="B24">
         <v>8906.3333333333339</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A25" s="3">
+      <c r="A25">
         <v>8483.75</v>
       </c>
-      <c r="B25" s="3">
+      <c r="B25">
         <v>8872.25</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A26" s="3">
+      <c r="A26">
         <v>8741.3333333333339</v>
       </c>
-      <c r="B26" s="3">
+      <c r="B26">
         <v>8943</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A27" s="3">
+      <c r="A27">
         <v>8633.3333333333339</v>
       </c>
-      <c r="B27" s="3">
+      <c r="B27">
         <v>8918</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A28" s="3">
+      <c r="A28">
         <v>8523.25</v>
       </c>
-      <c r="B28" s="3">
+      <c r="B28">
         <v>8777</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A29" s="3">
+      <c r="A29">
         <v>8660</v>
       </c>
-      <c r="B29" s="3">
+      <c r="B29">
         <v>8835.3333333333339</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A30" s="3">
+      <c r="A30">
         <v>8746.75</v>
       </c>
-      <c r="B30" s="3">
+      <c r="B30">
         <v>8936</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A31" s="3">
+      <c r="A31">
         <v>8564.6666666666661</v>
       </c>
-      <c r="B31" s="3">
+      <c r="B31">
         <v>8817.6666666666661</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A32" s="3">
+      <c r="A32">
         <v>8611.6666666666661</v>
       </c>
-      <c r="B32" s="3">
+      <c r="B32">
         <v>8792.6666666666661</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A33" s="3">
+      <c r="A33">
         <v>8637.25</v>
       </c>
-      <c r="B33" s="3">
+      <c r="B33">
         <v>8894.25</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A34" s="3">
+      <c r="A34">
         <v>8538</v>
       </c>
-      <c r="B34" s="3">
+      <c r="B34">
         <v>8781</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A35" s="3">
+      <c r="A35">
         <v>8557</v>
       </c>
-      <c r="B35" s="3">
+      <c r="B35">
         <v>8773</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A36" s="3">
+      <c r="A36">
         <v>8594.3333333333339</v>
       </c>
-      <c r="B36" s="3">
+      <c r="B36">
         <v>8862.6666666666661</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A37" s="3">
+      <c r="A37">
         <v>8548.25</v>
       </c>
-      <c r="B37" s="3">
+      <c r="B37">
         <v>8858.5</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A38" s="3">
+      <c r="A38">
         <v>8617</v>
       </c>
-      <c r="B38" s="3">
+      <c r="B38">
         <v>8904.3333333333339</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A39" s="3">
+      <c r="A39">
         <v>8699.25</v>
       </c>
-      <c r="B39" s="3">
+      <c r="B39">
         <v>8835.25</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A40" s="3">
+      <c r="A40">
         <v>12269.75</v>
       </c>
-      <c r="B40" s="3">
+      <c r="B40">
         <v>12348.5</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A41" s="3">
+      <c r="A41">
         <v>11024.333333333334</v>
       </c>
-      <c r="B41" s="3">
+      <c r="B41">
         <v>11244.666666666666</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A42" s="3">
+      <c r="A42">
         <v>9964.6666666666661</v>
       </c>
-      <c r="B42" s="3">
+      <c r="B42">
         <v>10324.666666666666</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A43" s="3">
+      <c r="A43">
         <v>8872.5</v>
       </c>
-      <c r="B43" s="3">
+      <c r="B43">
         <v>9451.75</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A44" s="3">
+      <c r="A44">
         <v>8082.666666666667</v>
       </c>
-      <c r="B44" s="3">
+      <c r="B44">
         <v>8662</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A45" s="3">
+      <c r="A45">
         <v>8244</v>
       </c>
-      <c r="B45" s="3">
+      <c r="B45">
         <v>8498</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A46" s="3">
+      <c r="A46">
         <v>8788.0400000000009</v>
       </c>
-      <c r="B46" s="3">
+      <c r="B46">
         <v>9046.1466666666674</v>
       </c>
     </row>

</xml_diff>